<commit_message>
Update excel_file variable to 'Cariboo_replacement_jobs_2_of2.xlsx' in autoast_v2_Cuisinart_DEV.py
Working throught trapline boundaries script
</commit_message>
<xml_diff>
--- a/autoast/Cariboo_replacement_jobs_2_of2.xlsx
+++ b/autoast/Cariboo_replacement_jobs_2_of2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="27945" windowHeight="10875" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ast_config" sheetId="1" state="visible" r:id="rId1"/>
@@ -119,19 +119,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
@@ -530,11 +530,11 @@
   </sheetPr>
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="23.5703125" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="138.85546875" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
@@ -632,25 +632,24 @@
           <t>Cariboo</t>
         </is>
       </c>
-      <c r="B2" s="12" t="n"/>
       <c r="C2" s="6" t="inlineStr">
         <is>
-          <t>3401258</t>
+          <t>5401115</t>
         </is>
       </c>
       <c r="D2" s="6" t="inlineStr">
         <is>
-          <t>950591</t>
+          <t xml:space="preserve">      950246</t>
         </is>
       </c>
       <c r="E2" s="6" t="inlineStr">
         <is>
-          <t>985890</t>
+          <t>985354</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>\\spatialfiles.bcgov\work\srm\wml\Workarea\Authorizations\Land\Cariboo\3401258\Status_Nov2024</t>
+          <t>\\spatialfiles.bcgov\work\srm\wml\Workarea\Authorizations\Land\Cariboo\5401115\Status_Nov2024</t>
         </is>
       </c>
       <c r="G2" s="7" t="inlineStr">
@@ -683,13 +682,11 @@
           <t>true</t>
         </is>
       </c>
-      <c r="M2" s="11" t="inlineStr">
-        <is>
-          <t>COMPLETE</t>
-        </is>
-      </c>
-      <c r="N2" s="12" t="n"/>
-      <c r="O2" s="2" t="n"/>
+      <c r="M2" s="13" t="inlineStr">
+        <is>
+          <t>Failed</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="19.5" customHeight="1" s="5">
       <c r="A3" s="2" t="inlineStr">
@@ -697,25 +694,25 @@
           <t>Cariboo</t>
         </is>
       </c>
-      <c r="B3" s="10" t="n"/>
+      <c r="B3" s="9" t="n"/>
       <c r="C3" s="6" t="inlineStr">
         <is>
-          <t>3411535</t>
+          <t>3401258</t>
         </is>
       </c>
       <c r="D3" s="6" t="inlineStr">
         <is>
-          <t>950592</t>
+          <t>950591</t>
         </is>
       </c>
       <c r="E3" s="6" t="inlineStr">
         <is>
-          <t>985891</t>
+          <t>985890</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>\\spatialfiles.bcgov\work\srm\wml\Workarea\Authorizations\Land\Cariboo\3411535\Status_Nov2024</t>
+          <t>\\spatialfiles.bcgov\work\srm\wml\Workarea\Authorizations\Land\Cariboo\3401258\Status_Nov2024</t>
         </is>
       </c>
       <c r="G3" s="7" t="inlineStr">
@@ -748,13 +745,13 @@
           <t>true</t>
         </is>
       </c>
-      <c r="M3" s="11" t="inlineStr">
-        <is>
-          <t>COMPLETE</t>
-        </is>
-      </c>
-      <c r="N3" s="13" t="n"/>
-      <c r="O3" s="8" t="n"/>
+      <c r="M3" s="10" t="inlineStr">
+        <is>
+          <t>Queued</t>
+        </is>
+      </c>
+      <c r="N3" s="9" t="n"/>
+      <c r="O3" s="2" t="n"/>
     </row>
     <row r="4" ht="19.5" customHeight="1" s="5">
       <c r="A4" s="2" t="inlineStr">
@@ -762,24 +759,25 @@
           <t>Cariboo</t>
         </is>
       </c>
+      <c r="B4" s="11" t="n"/>
       <c r="C4" s="6" t="inlineStr">
         <is>
-          <t>5401115</t>
+          <t>3411535</t>
         </is>
       </c>
       <c r="D4" s="6" t="inlineStr">
         <is>
-          <t>950246</t>
+          <t>950592</t>
         </is>
       </c>
       <c r="E4" s="6" t="inlineStr">
         <is>
-          <t>985354</t>
+          <t>985891</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>\\spatialfiles.bcgov\work\srm\wml\Workarea\Authorizations\Land\Cariboo\5401115\Status_Nov2024</t>
+          <t>\\spatialfiles.bcgov\work\srm\wml\Workarea\Authorizations\Land\Cariboo\3411535\Status_Nov2024</t>
         </is>
       </c>
       <c r="G4" s="7" t="inlineStr">
@@ -812,11 +810,13 @@
           <t>true</t>
         </is>
       </c>
-      <c r="M4" s="9" t="inlineStr">
-        <is>
-          <t>COMPLETE</t>
-        </is>
-      </c>
+      <c r="M4" s="10" t="inlineStr">
+        <is>
+          <t>Queued</t>
+        </is>
+      </c>
+      <c r="N4" s="12" t="n"/>
+      <c r="O4" s="8" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -838,7 +838,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="27.140625" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="13.5703125" bestFit="1" customWidth="1" style="5" min="2" max="3"/>

</xml_diff>

<commit_message>
Created V2 of Fish and Wildlife toolbox to start over need to start with file paths
</commit_message>
<xml_diff>
--- a/autoast/Cariboo_replacement_jobs_2_of2.xlsx
+++ b/autoast/Cariboo_replacement_jobs_2_of2.xlsx
@@ -522,310 +522,6 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="23.5703125" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="138.85546875" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
-    <col width="17.7109375" bestFit="1" customWidth="1" style="14" min="3" max="3"/>
-    <col width="16.85546875" bestFit="1" customWidth="1" style="14" min="4" max="4"/>
-    <col width="17.28515625" bestFit="1" customWidth="1" style="14" min="5" max="5"/>
-    <col width="110.42578125" bestFit="1" customWidth="1" style="4" min="6" max="6"/>
-    <col width="29.28515625" bestFit="1" customWidth="1" style="15" min="7" max="7"/>
-    <col width="20.5703125" bestFit="1" customWidth="1" style="15" min="8" max="8"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="15" min="9" max="9"/>
-    <col width="21" bestFit="1" customWidth="1" style="15" min="10" max="10"/>
-    <col width="21.28515625" bestFit="1" customWidth="1" style="15" min="11" max="11"/>
-    <col width="13.7109375" bestFit="1" customWidth="1" style="15" min="12" max="12"/>
-    <col width="14.7109375" bestFit="1" customWidth="1" style="5" min="13" max="13"/>
-    <col width="11.5703125" bestFit="1" customWidth="1" style="5" min="14" max="14"/>
-    <col width="13.5703125" bestFit="1" customWidth="1" style="5" min="15" max="15"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="19.5" customHeight="1" s="5">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>region</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>feature_layer</t>
-        </is>
-      </c>
-      <c r="C1" s="6" t="inlineStr">
-        <is>
-          <t>crown_file_number</t>
-        </is>
-      </c>
-      <c r="D1" s="6" t="inlineStr">
-        <is>
-          <t>disposition_number</t>
-        </is>
-      </c>
-      <c r="E1" s="6" t="inlineStr">
-        <is>
-          <t>parcel_number</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>output_directory</t>
-        </is>
-      </c>
-      <c r="G1" s="7" t="inlineStr">
-        <is>
-          <t>output_directory_same_as_input</t>
-        </is>
-      </c>
-      <c r="H1" s="7" t="inlineStr">
-        <is>
-          <t>dont_overwrite_outputs</t>
-        </is>
-      </c>
-      <c r="I1" s="7" t="inlineStr">
-        <is>
-          <t>skip_conflicts_and_constraints</t>
-        </is>
-      </c>
-      <c r="J1" s="7" t="inlineStr">
-        <is>
-          <t>suppress_map_creation</t>
-        </is>
-      </c>
-      <c r="K1" s="7" t="inlineStr">
-        <is>
-          <t>add_maps_to_current</t>
-        </is>
-      </c>
-      <c r="L1" s="7" t="inlineStr">
-        <is>
-          <t>run_as_fcbc</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="inlineStr">
-        <is>
-          <t>ast_condition</t>
-        </is>
-      </c>
-      <c r="N1" s="8" t="inlineStr">
-        <is>
-          <t>file_number</t>
-        </is>
-      </c>
-      <c r="O1" s="8" t="n"/>
-    </row>
-    <row r="2" ht="19.5" customHeight="1" s="5">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>Cariboo</t>
-        </is>
-      </c>
-      <c r="C2" s="6" t="inlineStr">
-        <is>
-          <t>5401115</t>
-        </is>
-      </c>
-      <c r="D2" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">      950246</t>
-        </is>
-      </c>
-      <c r="E2" s="6" t="inlineStr">
-        <is>
-          <t>985354</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>\\spatialfiles.bcgov\work\srm\wml\Workarea\Authorizations\Land\Cariboo\5401115\Status_Nov2024</t>
-        </is>
-      </c>
-      <c r="G2" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H2" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I2" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J2" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K2" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L2" s="7" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="M2" s="13" t="inlineStr">
-        <is>
-          <t>Failed</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="19.5" customHeight="1" s="5">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Cariboo</t>
-        </is>
-      </c>
-      <c r="B3" s="9" t="n"/>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>3401258</t>
-        </is>
-      </c>
-      <c r="D3" s="6" t="inlineStr">
-        <is>
-          <t>950591</t>
-        </is>
-      </c>
-      <c r="E3" s="6" t="inlineStr">
-        <is>
-          <t>985890</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>\\spatialfiles.bcgov\work\srm\wml\Workarea\Authorizations\Land\Cariboo\3401258\Status_Nov2024</t>
-        </is>
-      </c>
-      <c r="G3" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H3" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I3" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J3" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K3" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L3" s="7" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="M3" s="10" t="inlineStr">
-        <is>
-          <t>Queued</t>
-        </is>
-      </c>
-      <c r="N3" s="9" t="n"/>
-      <c r="O3" s="2" t="n"/>
-    </row>
-    <row r="4" ht="19.5" customHeight="1" s="5">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Cariboo</t>
-        </is>
-      </c>
-      <c r="B4" s="11" t="n"/>
-      <c r="C4" s="6" t="inlineStr">
-        <is>
-          <t>3411535</t>
-        </is>
-      </c>
-      <c r="D4" s="6" t="inlineStr">
-        <is>
-          <t>950592</t>
-        </is>
-      </c>
-      <c r="E4" s="6" t="inlineStr">
-        <is>
-          <t>985891</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>\\spatialfiles.bcgov\work\srm\wml\Workarea\Authorizations\Land\Cariboo\3411535\Status_Nov2024</t>
-        </is>
-      </c>
-      <c r="G4" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="H4" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="I4" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="J4" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="K4" s="7" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-      <c r="L4" s="7" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="M4" s="10" t="inlineStr">
-        <is>
-          <t>Queued</t>
-        </is>
-      </c>
-      <c r="N4" s="12" t="n"/>
-      <c r="O4" s="8" t="n"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -838,7 +534,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="27.140625" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
     <col width="13.5703125" bestFit="1" customWidth="1" style="5" min="2" max="3"/>

</xml_diff>